<commit_message>
speech classes ready for testing
</commit_message>
<xml_diff>
--- a/dialogue/Hello World Example/1-Hello-World (2).xlsx
+++ b/dialogue/Hello World Example/1-Hello-World (2).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin Gagich\Documents\GitHub\hitchBOT\dialogue\Hello World Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dom\workspace\hitchBOT\dialogue\Hello World Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>Type</t>
   </si>
@@ -199,13 +199,37 @@
   </si>
   <si>
     <t>mode=none &amp; lm=001</t>
+  </si>
+  <si>
+    <t>in_audio</t>
+  </si>
+  <si>
+    <t>tell me a story please please</t>
+  </si>
+  <si>
+    <t>out_story</t>
+  </si>
+  <si>
+    <t>Would you like me to tell you a story?</t>
+  </si>
+  <si>
+    <t>in_yes</t>
+  </si>
+  <si>
+    <t>in_no</t>
+  </si>
+  <si>
+    <t>yes /  ok / yeah</t>
+  </si>
+  <si>
+    <t>no / nope / nah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -310,6 +334,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -497,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -538,6 +568,10 @@
     <xf numFmtId="0" fontId="17" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,27 +852,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.1328125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" customWidth="1"/>
+    <col min="3" max="3" width="7.265625" customWidth="1"/>
+    <col min="4" max="4" width="135.1328125" customWidth="1"/>
+    <col min="5" max="5" width="15.9296875" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" customWidth="1"/>
+    <col min="7" max="7" width="14.265625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -867,7 +901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -886,7 +920,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>12</v>
       </c>
@@ -907,7 +941,7 @@
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -924,7 +958,7 @@
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
@@ -945,166 +979,174 @@
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
+      <c r="D6" s="23" t="s">
+        <v>61</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H6" s="1">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="23" t="s">
-        <v>23</v>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1">
         <v>70</v>
       </c>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>26</v>
+      <c r="D8" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H8" s="1">
         <v>70</v>
       </c>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1">
+        <v>70</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H11" s="13">
         <v>100</v>
       </c>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="8" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -1112,65 +1154,61 @@
       <c r="H14" s="18"/>
       <c r="I14" s="15"/>
     </row>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="8" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
+    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
@@ -1178,81 +1216,81 @@
       <c r="H18" s="19"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H20" s="1">
         <v>70</v>
       </c>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H21" s="4">
         <v>70</v>
       </c>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
@@ -1260,41 +1298,95 @@
       <c r="H22" s="19"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="19"/>
+    <row r="24" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
       <c r="I24" s="8"/>
     </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>